<commit_message>
Implimented white box functions, corrected an error with valid function, updated matrix
</commit_message>
<xml_diff>
--- a/Documents/Testing/TestDocuments/traceability-matrix-g3.xlsx
+++ b/Documents/Testing/TestDocuments/traceability-matrix-g3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ntg18\Documents\GitHub\winter25-sft221-nee-3\Documents\Testing\TestDocuments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D850E38-4F88-4C3D-9678-22C3B3E1C2DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D75AF0C5-78CC-4D29-954D-F349A2E5C7E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{2BF2C2EA-6658-4885-BCA1-B03AABC6ADA8}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="52">
   <si>
     <t>Requirements Traceability Matrix</t>
   </si>
@@ -85,12 +85,6 @@
     <t>UAT</t>
   </si>
   <si>
-    <t>WT01</t>
-  </si>
-  <si>
-    <t>WT02</t>
-  </si>
-  <si>
     <t>IT01</t>
   </si>
   <si>
@@ -100,12 +94,6 @@
     <t>Test ID</t>
   </si>
   <si>
-    <t>WT03</t>
-  </si>
-  <si>
-    <t>WT04</t>
-  </si>
-  <si>
     <t>UAT01</t>
   </si>
   <si>
@@ -155,6 +143,54 @@
   </si>
   <si>
     <t>R008</t>
+  </si>
+  <si>
+    <t>test_checkSpace1</t>
+  </si>
+  <si>
+    <t>test_checkSpace2</t>
+  </si>
+  <si>
+    <t>test_checkSpace3</t>
+  </si>
+  <si>
+    <t>test_checkSpace4</t>
+  </si>
+  <si>
+    <t>test_valid1</t>
+  </si>
+  <si>
+    <t>test_valid2</t>
+  </si>
+  <si>
+    <t>test_valid3</t>
+  </si>
+  <si>
+    <t>test_valid4</t>
+  </si>
+  <si>
+    <t>test_assign1</t>
+  </si>
+  <si>
+    <t>test_assign2</t>
+  </si>
+  <si>
+    <t>test_assign3</t>
+  </si>
+  <si>
+    <t>test_assign4</t>
+  </si>
+  <si>
+    <t>test_max1</t>
+  </si>
+  <si>
+    <t>test_max2</t>
+  </si>
+  <si>
+    <t>test_max3</t>
+  </si>
+  <si>
+    <t>test_max4</t>
   </si>
 </sst>
 </file>
@@ -176,7 +212,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -234,6 +270,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF8B8B"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -302,7 +356,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -317,6 +371,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -335,12 +395,9 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -660,46 +717,47 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BF1E143-845D-46A9-96E7-D791D2617AEF}">
-  <dimension ref="A1:O39"/>
+  <dimension ref="A1:O51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="D42" sqref="D42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="19.54296875" customWidth="1"/>
-    <col min="2" max="3" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.26953125" customWidth="1"/>
+    <col min="3" max="3" width="12.453125" bestFit="1" customWidth="1"/>
     <col min="4" max="13" width="9.1796875" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="C1" s="11" t="s">
+      <c r="B1" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
-      <c r="J1" s="7"/>
-      <c r="K1" s="7"/>
-      <c r="L1" s="7"/>
-      <c r="M1" s="7"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="13"/>
+      <c r="K1" s="13"/>
+      <c r="L1" s="13"/>
+      <c r="M1" s="13"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A2" s="6"/>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
+      <c r="A2" s="12"/>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
       <c r="D2" s="2" t="s">
         <v>2</v>
       </c>
@@ -722,17 +780,17 @@
         <v>8</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="L2" s="2"/>
       <c r="M2" s="2"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="12" t="s">
-        <v>25</v>
+      <c r="B3" s="6" t="s">
+        <v>21</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>12</v>
@@ -751,9 +809,9 @@
       <c r="M3" s="5"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A4" s="9"/>
-      <c r="B4" s="12" t="s">
-        <v>25</v>
+      <c r="A4" s="15"/>
+      <c r="B4" s="6" t="s">
+        <v>21</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>12</v>
@@ -774,9 +832,9 @@
       <c r="M4" s="5"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A5" s="9"/>
-      <c r="B5" s="12" t="s">
-        <v>25</v>
+      <c r="A5" s="15"/>
+      <c r="B5" s="6" t="s">
+        <v>21</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>12</v>
@@ -795,9 +853,9 @@
       <c r="M5" s="5"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A6" s="9"/>
-      <c r="B6" s="12" t="s">
-        <v>25</v>
+      <c r="A6" s="15"/>
+      <c r="B6" s="6" t="s">
+        <v>21</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>12</v>
@@ -817,13 +875,13 @@
       <c r="L6" s="5"/>
       <c r="M6" s="5"/>
       <c r="O6" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A7" s="9"/>
-      <c r="B7" s="13" t="s">
-        <v>26</v>
+      <c r="A7" s="15"/>
+      <c r="B7" s="7" t="s">
+        <v>22</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>12</v>
@@ -845,13 +903,13 @@
       <c r="L7" s="5"/>
       <c r="M7" s="5"/>
       <c r="O7" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A8" s="9"/>
-      <c r="B8" s="13" t="s">
-        <v>26</v>
+      <c r="A8" s="15"/>
+      <c r="B8" s="7" t="s">
+        <v>22</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>12</v>
@@ -873,13 +931,13 @@
       <c r="L8" s="5"/>
       <c r="M8" s="5"/>
       <c r="O8" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A9" s="9"/>
-      <c r="B9" s="13" t="s">
-        <v>26</v>
+      <c r="A9" s="15"/>
+      <c r="B9" s="7" t="s">
+        <v>22</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>12</v>
@@ -901,13 +959,13 @@
       <c r="L9" s="5"/>
       <c r="M9" s="5"/>
       <c r="O9" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A10" s="9"/>
-      <c r="B10" s="13" t="s">
-        <v>26</v>
+      <c r="A10" s="15"/>
+      <c r="B10" s="7" t="s">
+        <v>22</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>12</v>
@@ -929,13 +987,13 @@
       <c r="L10" s="5"/>
       <c r="M10" s="5"/>
       <c r="O10" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A11" s="9"/>
-      <c r="B11" s="14" t="s">
-        <v>27</v>
+      <c r="A11" s="15"/>
+      <c r="B11" s="8" t="s">
+        <v>23</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>12</v>
@@ -955,13 +1013,13 @@
       <c r="L11" s="5"/>
       <c r="M11" s="5"/>
       <c r="O11" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A12" s="9"/>
-      <c r="B12" s="14" t="s">
-        <v>27</v>
+      <c r="A12" s="15"/>
+      <c r="B12" s="8" t="s">
+        <v>23</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>12</v>
@@ -983,13 +1041,13 @@
       <c r="L12" s="5"/>
       <c r="M12" s="5"/>
       <c r="O12" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A13" s="9"/>
-      <c r="B13" s="14" t="s">
-        <v>27</v>
+      <c r="A13" s="15"/>
+      <c r="B13" s="8" t="s">
+        <v>23</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>12</v>
@@ -1007,13 +1065,13 @@
       <c r="L13" s="5"/>
       <c r="M13" s="5"/>
       <c r="O13" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A14" s="9"/>
-      <c r="B14" s="14" t="s">
-        <v>27</v>
+      <c r="A14" s="15"/>
+      <c r="B14" s="8" t="s">
+        <v>23</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>12</v>
@@ -1036,9 +1094,9 @@
       <c r="M14" s="5"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A15" s="9"/>
-      <c r="B15" s="15" t="s">
-        <v>28</v>
+      <c r="A15" s="15"/>
+      <c r="B15" s="9" t="s">
+        <v>24</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>12</v>
@@ -1063,9 +1121,9 @@
       <c r="M15" s="5"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A16" s="9"/>
-      <c r="B16" s="15" t="s">
-        <v>28</v>
+      <c r="A16" s="15"/>
+      <c r="B16" s="9" t="s">
+        <v>24</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>12</v>
@@ -1084,9 +1142,9 @@
       <c r="M16" s="5"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A17" s="9"/>
-      <c r="B17" s="15" t="s">
-        <v>28</v>
+      <c r="A17" s="15"/>
+      <c r="B17" s="9" t="s">
+        <v>24</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>12</v>
@@ -1105,9 +1163,9 @@
       <c r="M17" s="5"/>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A18" s="9"/>
-      <c r="B18" s="15" t="s">
-        <v>28</v>
+      <c r="A18" s="15"/>
+      <c r="B18" s="9" t="s">
+        <v>24</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>12</v>
@@ -1126,9 +1184,9 @@
       <c r="M18" s="5"/>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A19" s="9"/>
-      <c r="B19" s="16" t="s">
-        <v>29</v>
+      <c r="A19" s="15"/>
+      <c r="B19" s="10" t="s">
+        <v>25</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>12</v>
@@ -1147,9 +1205,9 @@
       <c r="M19" s="5"/>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A20" s="9"/>
-      <c r="B20" s="16" t="s">
-        <v>29</v>
+      <c r="A20" s="15"/>
+      <c r="B20" s="10" t="s">
+        <v>25</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>12</v>
@@ -1168,9 +1226,9 @@
       <c r="M20" s="5"/>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A21" s="9"/>
-      <c r="B21" s="16" t="s">
-        <v>29</v>
+      <c r="A21" s="15"/>
+      <c r="B21" s="10" t="s">
+        <v>25</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>12</v>
@@ -1189,9 +1247,9 @@
       <c r="M21" s="5"/>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A22" s="9"/>
-      <c r="B22" s="16" t="s">
-        <v>29</v>
+      <c r="A22" s="15"/>
+      <c r="B22" s="10" t="s">
+        <v>25</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>12</v>
@@ -1212,9 +1270,9 @@
       <c r="M22" s="5"/>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A23" s="9"/>
-      <c r="B23" s="17" t="s">
-        <v>30</v>
+      <c r="A23" s="15"/>
+      <c r="B23" s="11" t="s">
+        <v>26</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>12</v>
@@ -1235,9 +1293,9 @@
       <c r="M23" s="5"/>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A24" s="9"/>
-      <c r="B24" s="17" t="s">
-        <v>30</v>
+      <c r="A24" s="15"/>
+      <c r="B24" s="11" t="s">
+        <v>26</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>12</v>
@@ -1256,9 +1314,9 @@
       <c r="M24" s="5"/>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A25" s="9"/>
-      <c r="B25" s="17" t="s">
-        <v>30</v>
+      <c r="A25" s="15"/>
+      <c r="B25" s="11" t="s">
+        <v>26</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>12</v>
@@ -1277,9 +1335,9 @@
       <c r="M25" s="5"/>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A26" s="9"/>
-      <c r="B26" s="17" t="s">
-        <v>30</v>
+      <c r="A26" s="15"/>
+      <c r="B26" s="11" t="s">
+        <v>26</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>12</v>
@@ -1298,16 +1356,22 @@
       <c r="M26" s="5"/>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A27" s="9"/>
+      <c r="A27" s="15"/>
       <c r="B27" s="1" t="s">
-        <v>16</v>
+        <v>36</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D27" s="5"/>
-      <c r="E27" s="5"/>
-      <c r="F27" s="5"/>
+      <c r="D27" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E27" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F27" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="G27" s="5"/>
       <c r="H27" s="5"/>
       <c r="I27" s="5"/>
@@ -1317,15 +1381,19 @@
       <c r="M27" s="5"/>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A28" s="9"/>
+      <c r="A28" s="15"/>
       <c r="B28" s="1" t="s">
-        <v>17</v>
+        <v>37</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D28" s="5"/>
-      <c r="E28" s="5"/>
+      <c r="D28" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E28" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="F28" s="5"/>
       <c r="G28" s="5"/>
       <c r="H28" s="5"/>
@@ -1336,15 +1404,19 @@
       <c r="M28" s="5"/>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A29" s="9"/>
+      <c r="A29" s="15"/>
       <c r="B29" s="1" t="s">
-        <v>21</v>
+        <v>38</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D29" s="5"/>
-      <c r="E29" s="5"/>
+      <c r="D29" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E29" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="F29" s="5"/>
       <c r="G29" s="5"/>
       <c r="H29" s="5"/>
@@ -1355,35 +1427,43 @@
       <c r="M29" s="5"/>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A30" s="9"/>
+      <c r="A30" s="15"/>
       <c r="B30" s="1" t="s">
-        <v>22</v>
+        <v>39</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D30" s="5"/>
-      <c r="E30" s="5"/>
+      <c r="E30" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="F30" s="5"/>
       <c r="G30" s="5"/>
       <c r="H30" s="5"/>
       <c r="I30" s="5"/>
-      <c r="J30" s="5"/>
+      <c r="J30" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="K30" s="5"/>
       <c r="L30" s="5"/>
       <c r="M30" s="5"/>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A31" s="9"/>
-      <c r="B31" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>14</v>
+      <c r="A31" s="15"/>
+      <c r="B31" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="C31" s="18" t="s">
+        <v>13</v>
       </c>
       <c r="D31" s="5"/>
-      <c r="E31" s="5"/>
-      <c r="F31" s="5"/>
+      <c r="E31" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F31" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="G31" s="5"/>
       <c r="H31" s="5"/>
       <c r="I31" s="5"/>
@@ -1393,15 +1473,19 @@
       <c r="M31" s="5"/>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A32" s="9"/>
-      <c r="B32" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D32" s="5"/>
-      <c r="E32" s="5"/>
+      <c r="A32" s="15"/>
+      <c r="B32" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="C32" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E32" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="F32" s="5"/>
       <c r="G32" s="5"/>
       <c r="H32" s="5"/>
@@ -1412,18 +1496,20 @@
       <c r="M32" s="5"/>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A33" s="9"/>
-      <c r="B33" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>15</v>
+      <c r="A33" s="15"/>
+      <c r="B33" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="C33" s="18" t="s">
+        <v>13</v>
       </c>
       <c r="D33" s="5"/>
       <c r="E33" s="5"/>
       <c r="F33" s="5"/>
       <c r="G33" s="5"/>
-      <c r="H33" s="5"/>
+      <c r="H33" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="I33" s="5"/>
       <c r="J33" s="5"/>
       <c r="K33" s="5"/>
@@ -1431,36 +1517,293 @@
       <c r="M33" s="5"/>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A34" s="10"/>
-      <c r="B34" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>15</v>
+      <c r="A34" s="15"/>
+      <c r="B34" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="C34" s="18" t="s">
+        <v>13</v>
       </c>
       <c r="D34" s="5"/>
       <c r="E34" s="5"/>
       <c r="F34" s="5"/>
       <c r="G34" s="5"/>
-      <c r="H34" s="5"/>
+      <c r="H34" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="I34" s="5"/>
       <c r="J34" s="5"/>
       <c r="K34" s="5"/>
       <c r="L34" s="5"/>
       <c r="M34" s="5"/>
     </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A35" s="15"/>
+      <c r="B35" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="C35" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="D35" s="5"/>
+      <c r="E35" s="5"/>
+      <c r="F35" s="5"/>
+      <c r="G35" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H35" s="5"/>
+      <c r="I35" s="5"/>
+      <c r="J35" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="K35" s="5"/>
+      <c r="L35" s="5"/>
+      <c r="M35" s="5"/>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A36" s="15"/>
+      <c r="B36" s="19" t="s">
+        <v>45</v>
+      </c>
+      <c r="C36" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="D36" s="5"/>
+      <c r="E36" s="5"/>
+      <c r="F36" s="5"/>
+      <c r="G36" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H36" s="5"/>
+      <c r="I36" s="5"/>
+      <c r="J36" s="5"/>
+      <c r="K36" s="5"/>
+      <c r="L36" s="5"/>
+      <c r="M36" s="5"/>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A37" s="15"/>
+      <c r="B37" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="C37" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="D37" s="5"/>
+      <c r="E37" s="5"/>
+      <c r="F37" s="5"/>
+      <c r="G37" s="5"/>
+      <c r="H37" s="5"/>
+      <c r="I37" s="5"/>
+      <c r="J37" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="K37" s="5"/>
+      <c r="L37" s="5"/>
+      <c r="M37" s="5"/>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A38" s="15"/>
+      <c r="B38" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="C38" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="D38" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E38" s="5"/>
+      <c r="F38" s="5"/>
+      <c r="G38" s="5"/>
+      <c r="H38" s="5"/>
+      <c r="I38" s="5"/>
+      <c r="J38" s="5"/>
+      <c r="K38" s="5"/>
+      <c r="L38" s="5"/>
+      <c r="M38" s="5"/>
+    </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="G39" s="4"/>
+      <c r="A39" s="15"/>
+      <c r="B39" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="C39" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="D39" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E39" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F39" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G39" s="5"/>
+      <c r="H39" s="5"/>
+      <c r="I39" s="5"/>
+      <c r="J39" s="5"/>
+      <c r="K39" s="5"/>
+      <c r="L39" s="5"/>
+      <c r="M39" s="5"/>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A40" s="15"/>
+      <c r="B40" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="C40" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="D40" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E40" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F40" s="5"/>
+      <c r="G40" s="5"/>
+      <c r="H40" s="5"/>
+      <c r="I40" s="5"/>
+      <c r="J40" s="5"/>
+      <c r="K40" s="5"/>
+      <c r="L40" s="5"/>
+      <c r="M40" s="5"/>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A41" s="15"/>
+      <c r="B41" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="C41" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="D41" s="5"/>
+      <c r="E41" s="5"/>
+      <c r="F41" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G41" s="5"/>
+      <c r="H41" s="5"/>
+      <c r="I41" s="5"/>
+      <c r="J41" s="5"/>
+      <c r="K41" s="5"/>
+      <c r="L41" s="5"/>
+      <c r="M41" s="5"/>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A42" s="15"/>
+      <c r="B42" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="C42" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="D42" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E42" s="5"/>
+      <c r="F42" s="5"/>
+      <c r="G42" s="5"/>
+      <c r="H42" s="5"/>
+      <c r="I42" s="5"/>
+      <c r="J42" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="K42" s="5"/>
+      <c r="L42" s="5"/>
+      <c r="M42" s="5"/>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A43" s="15"/>
+      <c r="B43" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D43" s="5"/>
+      <c r="E43" s="5"/>
+      <c r="F43" s="5"/>
+      <c r="G43" s="5"/>
+      <c r="H43" s="5"/>
+      <c r="I43" s="5"/>
+      <c r="J43" s="5"/>
+      <c r="K43" s="5"/>
+      <c r="L43" s="5"/>
+      <c r="M43" s="5"/>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A44" s="15"/>
+      <c r="B44" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D44" s="5"/>
+      <c r="E44" s="5"/>
+      <c r="F44" s="5"/>
+      <c r="G44" s="5"/>
+      <c r="H44" s="5"/>
+      <c r="I44" s="5"/>
+      <c r="J44" s="5"/>
+      <c r="K44" s="5"/>
+      <c r="L44" s="5"/>
+      <c r="M44" s="5"/>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A45" s="15"/>
+      <c r="B45" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D45" s="5"/>
+      <c r="E45" s="5"/>
+      <c r="F45" s="5"/>
+      <c r="G45" s="5"/>
+      <c r="H45" s="5"/>
+      <c r="I45" s="5"/>
+      <c r="J45" s="5"/>
+      <c r="K45" s="5"/>
+      <c r="L45" s="5"/>
+      <c r="M45" s="5"/>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A46" s="16"/>
+      <c r="B46" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D46" s="5"/>
+      <c r="E46" s="5"/>
+      <c r="F46" s="5"/>
+      <c r="G46" s="5"/>
+      <c r="H46" s="5"/>
+      <c r="I46" s="5"/>
+      <c r="J46" s="5"/>
+      <c r="K46" s="5"/>
+      <c r="L46" s="5"/>
+      <c r="M46" s="5"/>
+    </row>
+    <row r="51" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G51" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="D1:M1"/>
-    <mergeCell ref="A3:A34"/>
+    <mergeCell ref="A3:A46"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="B1:B2"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated matrix with the integration test cases and the acceptance test cases
</commit_message>
<xml_diff>
--- a/Documents/Testing/TestDocuments/traceability-matrix-g3.xlsx
+++ b/Documents/Testing/TestDocuments/traceability-matrix-g3.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kaitl\OneDrive\Documents\CANADA\SENECA\ALL COURSES\SEMESTER 2\SFT221\PROJECT\winter25-sft221-nee-3\Documents\Testing\TestDocuments\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ntg18\Documents\GitHub\winter25-sft221-nee-3\Documents\Testing\TestDocuments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31DF5DFF-4C92-4091-A39A-27FEE7661AE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2086389-C552-4B64-B6B6-B5627D6DEE2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{2BF2C2EA-6658-4885-BCA1-B03AABC6ADA8}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{2BF2C2EA-6658-4885-BCA1-B03AABC6ADA8}"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="2" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="93">
   <si>
     <t>Requirements Traceability Matrix</t>
   </si>
@@ -72,39 +72,9 @@
     <t>Integration</t>
   </si>
   <si>
-    <t>UAT</t>
-  </si>
-  <si>
-    <t>IT01</t>
-  </si>
-  <si>
-    <t>IT02</t>
-  </si>
-  <si>
     <t>Test ID</t>
   </si>
   <si>
-    <t>UAT01</t>
-  </si>
-  <si>
-    <t>UAT02</t>
-  </si>
-  <si>
-    <t>assignPackage</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test valid </t>
-  </si>
-  <si>
-    <t xml:space="preserve">checkSpace </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test divert </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test distance </t>
-  </si>
-  <si>
     <t>R001 = max weight on truck</t>
   </si>
   <si>
@@ -132,55 +102,208 @@
     <t>R008</t>
   </si>
   <si>
-    <t>test_checkSpace1</t>
-  </si>
-  <si>
-    <t>test_checkSpace2</t>
-  </si>
-  <si>
-    <t>test_checkSpace3</t>
-  </si>
-  <si>
-    <t>test_checkSpace4</t>
-  </si>
-  <si>
-    <t>test_valid1</t>
-  </si>
-  <si>
-    <t>test_valid2</t>
-  </si>
-  <si>
-    <t>test_valid3</t>
-  </si>
-  <si>
-    <t>test_valid4</t>
-  </si>
-  <si>
-    <t>test_assign1</t>
-  </si>
-  <si>
-    <t>test_assign2</t>
-  </si>
-  <si>
-    <t>test_assign3</t>
-  </si>
-  <si>
-    <t>test_assign4</t>
-  </si>
-  <si>
-    <t>test_max1</t>
-  </si>
-  <si>
-    <t>test_max2</t>
-  </si>
-  <si>
-    <t>test_max3</t>
-  </si>
-  <si>
-    <t>test_max4</t>
-  </si>
-  <si>
-    <t>Test eqPt</t>
+    <t>IT101</t>
+  </si>
+  <si>
+    <t>IT102</t>
+  </si>
+  <si>
+    <t>IT103</t>
+  </si>
+  <si>
+    <t>IT104</t>
+  </si>
+  <si>
+    <t>IT201</t>
+  </si>
+  <si>
+    <t>IT202</t>
+  </si>
+  <si>
+    <t>IT203</t>
+  </si>
+  <si>
+    <t>IT204</t>
+  </si>
+  <si>
+    <t>IT301</t>
+  </si>
+  <si>
+    <t>IT302</t>
+  </si>
+  <si>
+    <t>IT303</t>
+  </si>
+  <si>
+    <t>IT304</t>
+  </si>
+  <si>
+    <t>IT401</t>
+  </si>
+  <si>
+    <t>IT402</t>
+  </si>
+  <si>
+    <t>IT403</t>
+  </si>
+  <si>
+    <t>IT404</t>
+  </si>
+  <si>
+    <t>AT101</t>
+  </si>
+  <si>
+    <t>BT101</t>
+  </si>
+  <si>
+    <t>BT102</t>
+  </si>
+  <si>
+    <t>BT103</t>
+  </si>
+  <si>
+    <t>BT104</t>
+  </si>
+  <si>
+    <t>BT201</t>
+  </si>
+  <si>
+    <t>BT202</t>
+  </si>
+  <si>
+    <t>BT203</t>
+  </si>
+  <si>
+    <t>BT204</t>
+  </si>
+  <si>
+    <t>BT301</t>
+  </si>
+  <si>
+    <t>BT302</t>
+  </si>
+  <si>
+    <t>BT303</t>
+  </si>
+  <si>
+    <t>BT304</t>
+  </si>
+  <si>
+    <t>BT401</t>
+  </si>
+  <si>
+    <t>BT402</t>
+  </si>
+  <si>
+    <t>BT403</t>
+  </si>
+  <si>
+    <t>BT404</t>
+  </si>
+  <si>
+    <t>BT501</t>
+  </si>
+  <si>
+    <t>BT502</t>
+  </si>
+  <si>
+    <t>BT503</t>
+  </si>
+  <si>
+    <t>BT504</t>
+  </si>
+  <si>
+    <t>BT601</t>
+  </si>
+  <si>
+    <t>BT602</t>
+  </si>
+  <si>
+    <t>BT603</t>
+  </si>
+  <si>
+    <t>BT604</t>
+  </si>
+  <si>
+    <t>WT101</t>
+  </si>
+  <si>
+    <t>WT102</t>
+  </si>
+  <si>
+    <t>WT103</t>
+  </si>
+  <si>
+    <t>WT104</t>
+  </si>
+  <si>
+    <t>WT201</t>
+  </si>
+  <si>
+    <t>WT202</t>
+  </si>
+  <si>
+    <t>WT203</t>
+  </si>
+  <si>
+    <t>WT204</t>
+  </si>
+  <si>
+    <t>WT301</t>
+  </si>
+  <si>
+    <t>WT302</t>
+  </si>
+  <si>
+    <t>WT303</t>
+  </si>
+  <si>
+    <t>WT304</t>
+  </si>
+  <si>
+    <t>WT401</t>
+  </si>
+  <si>
+    <t>WT402</t>
+  </si>
+  <si>
+    <t>WT403</t>
+  </si>
+  <si>
+    <t>WT404</t>
+  </si>
+  <si>
+    <t>AT201</t>
+  </si>
+  <si>
+    <t>AT202</t>
+  </si>
+  <si>
+    <t>AT301</t>
+  </si>
+  <si>
+    <t>AT401</t>
+  </si>
+  <si>
+    <t>AT501</t>
+  </si>
+  <si>
+    <t>AT502</t>
+  </si>
+  <si>
+    <t>AT503</t>
+  </si>
+  <si>
+    <t>AT601</t>
+  </si>
+  <si>
+    <t>AT701</t>
+  </si>
+  <si>
+    <t>AT801</t>
+  </si>
+  <si>
+    <t>Acceptance</t>
   </si>
 </sst>
 </file>
@@ -202,7 +325,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="15">
+  <fills count="21">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -287,8 +410,44 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39994506668294322"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39994506668294322"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -335,24 +494,11 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -376,6 +522,9 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -388,13 +537,17 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -420,9 +573,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -460,7 +613,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -566,7 +719,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -708,7 +861,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -716,45 +869,45 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BF1E143-845D-46A9-96E7-D791D2617AEF}">
-  <dimension ref="A1:O51"/>
+  <dimension ref="A1:O74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="D54" sqref="D54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.5546875" customWidth="1"/>
-    <col min="2" max="2" width="17.21875" customWidth="1"/>
-    <col min="3" max="3" width="12.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="13" width="9.21875" style="3"/>
+    <col min="1" max="1" width="19.54296875" customWidth="1"/>
+    <col min="2" max="2" width="17.1796875" customWidth="1"/>
+    <col min="3" max="3" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="13" width="9.1796875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A1" s="15" t="s">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="20" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C1" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="16" t="s">
+      <c r="D1" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
-      <c r="J1" s="16"/>
-      <c r="K1" s="16"/>
-      <c r="L1" s="16"/>
-      <c r="M1" s="16"/>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A2" s="15"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17"/>
+      <c r="K1" s="17"/>
+      <c r="L1" s="17"/>
+      <c r="M1" s="17"/>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A2" s="16"/>
       <c r="B2" s="20"/>
       <c r="C2" s="20"/>
       <c r="D2" s="2" t="s">
@@ -779,17 +932,17 @@
         <v>8</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="L2" s="2"/>
       <c r="M2" s="2"/>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A3" s="17" t="s">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A3" s="18" t="s">
         <v>9</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>21</v>
+        <v>42</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>12</v>
@@ -798,7 +951,7 @@
       <c r="E3" s="5"/>
       <c r="F3" s="5"/>
       <c r="G3" s="5"/>
-      <c r="H3" s="21" t="s">
+      <c r="H3" s="15" t="s">
         <v>10</v>
       </c>
       <c r="I3" s="5"/>
@@ -807,10 +960,10 @@
       <c r="L3" s="5"/>
       <c r="M3" s="5"/>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A4" s="18"/>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A4" s="19"/>
       <c r="B4" s="6" t="s">
-        <v>21</v>
+        <v>43</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>12</v>
@@ -820,20 +973,20 @@
       <c r="F4" s="5"/>
       <c r="G4" s="5"/>
       <c r="H4" s="5"/>
-      <c r="I4" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="J4" s="21" t="s">
+      <c r="I4" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="J4" s="15" t="s">
         <v>10</v>
       </c>
       <c r="K4" s="5"/>
       <c r="L4" s="5"/>
       <c r="M4" s="5"/>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A5" s="18"/>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A5" s="19"/>
       <c r="B5" s="6" t="s">
-        <v>21</v>
+        <v>44</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>12</v>
@@ -842,7 +995,7 @@
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
       <c r="G5" s="5"/>
-      <c r="H5" s="21" t="s">
+      <c r="H5" s="15" t="s">
         <v>10</v>
       </c>
       <c r="I5" s="5"/>
@@ -851,10 +1004,10 @@
       <c r="L5" s="5"/>
       <c r="M5" s="5"/>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A6" s="18"/>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A6" s="19"/>
       <c r="B6" s="6" t="s">
-        <v>21</v>
+        <v>45</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>12</v>
@@ -864,64 +1017,64 @@
       <c r="F6" s="5"/>
       <c r="G6" s="5"/>
       <c r="H6" s="5"/>
-      <c r="I6" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="J6" s="21" t="s">
+      <c r="I6" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="J6" s="15" t="s">
         <v>10</v>
       </c>
       <c r="K6" s="5"/>
       <c r="L6" s="5"/>
       <c r="M6" s="5"/>
       <c r="O6" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A7" s="18"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A7" s="19"/>
       <c r="B7" s="7" t="s">
-        <v>22</v>
+        <v>46</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D7" s="5"/>
-      <c r="E7" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="F7" s="21" t="s">
+      <c r="E7" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" s="15" t="s">
         <v>10</v>
       </c>
       <c r="G7" s="5"/>
       <c r="H7" s="5"/>
       <c r="I7" s="5"/>
-      <c r="J7" s="21" t="s">
+      <c r="J7" s="15" t="s">
         <v>10</v>
       </c>
       <c r="K7" s="5"/>
       <c r="L7" s="5"/>
       <c r="M7" s="5"/>
       <c r="O7" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A8" s="18"/>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A8" s="19"/>
       <c r="B8" s="7" t="s">
-        <v>22</v>
+        <v>47</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D8" s="5"/>
-      <c r="E8" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="F8" s="21" t="s">
+      <c r="E8" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8" s="15" t="s">
         <v>10</v>
       </c>
       <c r="G8" s="5"/>
-      <c r="H8" s="21" t="s">
+      <c r="H8" s="15" t="s">
         <v>10</v>
       </c>
       <c r="I8" s="5"/>
@@ -930,26 +1083,26 @@
       <c r="L8" s="5"/>
       <c r="M8" s="5"/>
       <c r="O8" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A9" s="18"/>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A9" s="19"/>
       <c r="B9" s="7" t="s">
-        <v>22</v>
+        <v>48</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D9" s="5"/>
-      <c r="E9" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="F9" s="21" t="s">
+      <c r="E9" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9" s="15" t="s">
         <v>10</v>
       </c>
       <c r="G9" s="5"/>
-      <c r="H9" s="21" t="s">
+      <c r="H9" s="15" t="s">
         <v>10</v>
       </c>
       <c r="I9" s="5"/>
@@ -958,26 +1111,26 @@
       <c r="L9" s="5"/>
       <c r="M9" s="5"/>
       <c r="O9" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A10" s="18"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A10" s="19"/>
       <c r="B10" s="7" t="s">
-        <v>22</v>
+        <v>49</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D10" s="5"/>
-      <c r="E10" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="F10" s="21" t="s">
+      <c r="E10" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="F10" s="15" t="s">
         <v>10</v>
       </c>
       <c r="G10" s="5"/>
-      <c r="H10" s="21" t="s">
+      <c r="H10" s="15" t="s">
         <v>10</v>
       </c>
       <c r="I10" s="5"/>
@@ -986,21 +1139,21 @@
       <c r="L10" s="5"/>
       <c r="M10" s="5"/>
       <c r="O10" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A11" s="18"/>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A11" s="19"/>
       <c r="B11" s="8" t="s">
-        <v>23</v>
+        <v>50</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="E11" s="21" t="s">
+      <c r="D11" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11" s="15" t="s">
         <v>10</v>
       </c>
       <c r="F11" s="5"/>
@@ -1012,47 +1165,47 @@
       <c r="L11" s="5"/>
       <c r="M11" s="5"/>
       <c r="O11" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A12" s="18"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A12" s="19"/>
       <c r="B12" s="8" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D12" s="21" t="s">
+      <c r="D12" s="15" t="s">
         <v>10</v>
       </c>
       <c r="E12" s="5"/>
-      <c r="F12" s="21" t="s">
+      <c r="F12" s="15" t="s">
         <v>10</v>
       </c>
       <c r="G12" s="5"/>
       <c r="H12" s="5"/>
       <c r="I12" s="5"/>
-      <c r="J12" s="21" t="s">
+      <c r="J12" s="15" t="s">
         <v>10</v>
       </c>
       <c r="K12" s="5"/>
       <c r="L12" s="5"/>
       <c r="M12" s="5"/>
       <c r="O12" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A13" s="18"/>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A13" s="19"/>
       <c r="B13" s="8" t="s">
-        <v>23</v>
+        <v>52</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D13" s="5"/>
-      <c r="E13" s="21" t="s">
+      <c r="E13" s="15" t="s">
         <v>10</v>
       </c>
       <c r="F13" s="5"/>
@@ -1064,53 +1217,53 @@
       <c r="L13" s="5"/>
       <c r="M13" s="5"/>
       <c r="O13" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A14" s="18"/>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A14" s="19"/>
       <c r="B14" s="8" t="s">
-        <v>23</v>
+        <v>53</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D14" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="E14" s="21" t="s">
+      <c r="D14" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="E14" s="15" t="s">
         <v>10</v>
       </c>
       <c r="F14" s="5"/>
       <c r="G14" s="5"/>
       <c r="H14" s="5"/>
       <c r="I14" s="5"/>
-      <c r="J14" s="21" t="s">
+      <c r="J14" s="15" t="s">
         <v>10</v>
       </c>
       <c r="K14" s="5"/>
       <c r="L14" s="5"/>
       <c r="M14" s="5"/>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A15" s="18"/>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A15" s="19"/>
       <c r="B15" s="9" t="s">
-        <v>24</v>
+        <v>54</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D15" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="E15" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="F15" s="21" t="s">
+      <c r="D15" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="E15" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="F15" s="15" t="s">
         <v>10</v>
       </c>
       <c r="G15" s="5"/>
-      <c r="H15" s="21" t="s">
+      <c r="H15" s="15" t="s">
         <v>10</v>
       </c>
       <c r="I15" s="5"/>
@@ -1119,10 +1272,10 @@
       <c r="L15" s="5"/>
       <c r="M15" s="5"/>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A16" s="18"/>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A16" s="19"/>
       <c r="B16" s="9" t="s">
-        <v>24</v>
+        <v>55</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>12</v>
@@ -1132,7 +1285,7 @@
       <c r="F16" s="5"/>
       <c r="G16" s="5"/>
       <c r="H16" s="5"/>
-      <c r="I16" s="21" t="s">
+      <c r="I16" s="15" t="s">
         <v>10</v>
       </c>
       <c r="J16" s="5"/>
@@ -1140,15 +1293,15 @@
       <c r="L16" s="5"/>
       <c r="M16" s="5"/>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A17" s="18"/>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A17" s="19"/>
       <c r="B17" s="9" t="s">
-        <v>24</v>
+        <v>56</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D17" s="21" t="s">
+      <c r="D17" s="15" t="s">
         <v>10</v>
       </c>
       <c r="E17" s="5"/>
@@ -1161,10 +1314,10 @@
       <c r="L17" s="5"/>
       <c r="M17" s="5"/>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A18" s="18"/>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A18" s="19"/>
       <c r="B18" s="9" t="s">
-        <v>24</v>
+        <v>57</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>12</v>
@@ -1173,7 +1326,7 @@
       <c r="E18" s="5"/>
       <c r="F18" s="5"/>
       <c r="G18" s="5"/>
-      <c r="H18" s="21" t="s">
+      <c r="H18" s="15" t="s">
         <v>10</v>
       </c>
       <c r="I18" s="5"/>
@@ -1182,10 +1335,10 @@
       <c r="L18" s="5"/>
       <c r="M18" s="5"/>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A19" s="18"/>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A19" s="19"/>
       <c r="B19" s="10" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>12</v>
@@ -1193,7 +1346,7 @@
       <c r="D19" s="5"/>
       <c r="E19" s="5"/>
       <c r="F19" s="5"/>
-      <c r="G19" s="21" t="s">
+      <c r="G19" s="15" t="s">
         <v>10</v>
       </c>
       <c r="H19" s="5"/>
@@ -1203,10 +1356,10 @@
       <c r="L19" s="5"/>
       <c r="M19" s="5"/>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A20" s="18"/>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A20" s="19"/>
       <c r="B20" s="10" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>12</v>
@@ -1214,7 +1367,7 @@
       <c r="D20" s="5"/>
       <c r="E20" s="5"/>
       <c r="F20" s="5"/>
-      <c r="G20" s="21" t="s">
+      <c r="G20" s="15" t="s">
         <v>10</v>
       </c>
       <c r="H20" s="5"/>
@@ -1224,10 +1377,10 @@
       <c r="L20" s="5"/>
       <c r="M20" s="5"/>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A21" s="18"/>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A21" s="19"/>
       <c r="B21" s="10" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>12</v>
@@ -1235,7 +1388,7 @@
       <c r="D21" s="5"/>
       <c r="E21" s="5"/>
       <c r="F21" s="5"/>
-      <c r="G21" s="21" t="s">
+      <c r="G21" s="15" t="s">
         <v>10</v>
       </c>
       <c r="H21" s="5"/>
@@ -1245,10 +1398,10 @@
       <c r="L21" s="5"/>
       <c r="M21" s="5"/>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A22" s="18"/>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A22" s="19"/>
       <c r="B22" s="10" t="s">
-        <v>51</v>
+        <v>61</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>12</v>
@@ -1256,7 +1409,7 @@
       <c r="D22" s="5"/>
       <c r="E22" s="5"/>
       <c r="F22" s="5"/>
-      <c r="G22" s="21" t="s">
+      <c r="G22" s="15" t="s">
         <v>10</v>
       </c>
       <c r="H22" s="5"/>
@@ -1266,10 +1419,10 @@
       <c r="L22" s="5"/>
       <c r="M22" s="5"/>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A23" s="18"/>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A23" s="19"/>
       <c r="B23" s="11" t="s">
-        <v>25</v>
+        <v>62</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>12</v>
@@ -1278,10 +1431,10 @@
       <c r="E23" s="5"/>
       <c r="F23" s="5"/>
       <c r="G23" s="5"/>
-      <c r="H23" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="I23" s="21" t="s">
+      <c r="H23" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="I23" s="15" t="s">
         <v>10</v>
       </c>
       <c r="J23" s="5"/>
@@ -1289,10 +1442,10 @@
       <c r="L23" s="5"/>
       <c r="M23" s="5"/>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A24" s="18"/>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A24" s="19"/>
       <c r="B24" s="11" t="s">
-        <v>25</v>
+        <v>63</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>12</v>
@@ -1300,7 +1453,7 @@
       <c r="D24" s="5"/>
       <c r="E24" s="5"/>
       <c r="F24" s="5"/>
-      <c r="G24" s="21" t="s">
+      <c r="G24" s="15" t="s">
         <v>10</v>
       </c>
       <c r="H24" s="5"/>
@@ -1310,10 +1463,10 @@
       <c r="L24" s="5"/>
       <c r="M24" s="5"/>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A25" s="18"/>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A25" s="19"/>
       <c r="B25" s="11" t="s">
-        <v>25</v>
+        <v>64</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>12</v>
@@ -1321,7 +1474,7 @@
       <c r="D25" s="5"/>
       <c r="E25" s="5"/>
       <c r="F25" s="5"/>
-      <c r="G25" s="21" t="s">
+      <c r="G25" s="15" t="s">
         <v>10</v>
       </c>
       <c r="H25" s="5"/>
@@ -1331,10 +1484,10 @@
       <c r="L25" s="5"/>
       <c r="M25" s="5"/>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A26" s="18"/>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A26" s="19"/>
       <c r="B26" s="11" t="s">
-        <v>25</v>
+        <v>65</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>12</v>
@@ -1342,7 +1495,7 @@
       <c r="D26" s="5"/>
       <c r="E26" s="5"/>
       <c r="F26" s="5"/>
-      <c r="G26" s="21" t="s">
+      <c r="G26" s="15" t="s">
         <v>10</v>
       </c>
       <c r="H26" s="5"/>
@@ -1352,21 +1505,21 @@
       <c r="L26" s="5"/>
       <c r="M26" s="5"/>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A27" s="18"/>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A27" s="19"/>
       <c r="B27" s="1" t="s">
-        <v>35</v>
+        <v>66</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D27" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="E27" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="F27" s="21" t="s">
+      <c r="D27" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="E27" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="F27" s="15" t="s">
         <v>10</v>
       </c>
       <c r="G27" s="5"/>
@@ -1377,18 +1530,18 @@
       <c r="L27" s="5"/>
       <c r="M27" s="5"/>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A28" s="18"/>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A28" s="19"/>
       <c r="B28" s="1" t="s">
-        <v>36</v>
+        <v>67</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D28" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="E28" s="21" t="s">
+      <c r="D28" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="E28" s="15" t="s">
         <v>10</v>
       </c>
       <c r="F28" s="5"/>
@@ -1400,18 +1553,18 @@
       <c r="L28" s="5"/>
       <c r="M28" s="5"/>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A29" s="18"/>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A29" s="19"/>
       <c r="B29" s="1" t="s">
-        <v>37</v>
+        <v>68</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D29" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="E29" s="21" t="s">
+      <c r="D29" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="E29" s="15" t="s">
         <v>10</v>
       </c>
       <c r="F29" s="5"/>
@@ -1423,42 +1576,42 @@
       <c r="L29" s="5"/>
       <c r="M29" s="5"/>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A30" s="18"/>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A30" s="19"/>
       <c r="B30" s="1" t="s">
-        <v>38</v>
+        <v>69</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D30" s="5"/>
-      <c r="E30" s="21" t="s">
+      <c r="E30" s="15" t="s">
         <v>10</v>
       </c>
       <c r="F30" s="5"/>
       <c r="G30" s="5"/>
       <c r="H30" s="5"/>
       <c r="I30" s="5"/>
-      <c r="J30" s="21" t="s">
+      <c r="J30" s="15" t="s">
         <v>10</v>
       </c>
       <c r="K30" s="5"/>
       <c r="L30" s="5"/>
       <c r="M30" s="5"/>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A31" s="18"/>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A31" s="19"/>
       <c r="B31" s="12" t="s">
-        <v>39</v>
+        <v>70</v>
       </c>
       <c r="C31" s="12" t="s">
         <v>13</v>
       </c>
       <c r="D31" s="5"/>
-      <c r="E31" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="F31" s="21" t="s">
+      <c r="E31" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="F31" s="15" t="s">
         <v>10</v>
       </c>
       <c r="G31" s="5"/>
@@ -1469,18 +1622,18 @@
       <c r="L31" s="5"/>
       <c r="M31" s="5"/>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A32" s="18"/>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A32" s="19"/>
       <c r="B32" s="12" t="s">
-        <v>40</v>
+        <v>71</v>
       </c>
       <c r="C32" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="D32" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="E32" s="21" t="s">
+      <c r="D32" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="E32" s="15" t="s">
         <v>10</v>
       </c>
       <c r="F32" s="5"/>
@@ -1492,10 +1645,10 @@
       <c r="L32" s="5"/>
       <c r="M32" s="5"/>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A33" s="18"/>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A33" s="19"/>
       <c r="B33" s="12" t="s">
-        <v>41</v>
+        <v>72</v>
       </c>
       <c r="C33" s="12" t="s">
         <v>13</v>
@@ -1504,7 +1657,7 @@
       <c r="E33" s="5"/>
       <c r="F33" s="5"/>
       <c r="G33" s="5"/>
-      <c r="H33" s="21" t="s">
+      <c r="H33" s="15" t="s">
         <v>10</v>
       </c>
       <c r="I33" s="5"/>
@@ -1513,10 +1666,10 @@
       <c r="L33" s="5"/>
       <c r="M33" s="5"/>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A34" s="18"/>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A34" s="19"/>
       <c r="B34" s="12" t="s">
-        <v>42</v>
+        <v>73</v>
       </c>
       <c r="C34" s="12" t="s">
         <v>13</v>
@@ -1525,7 +1678,7 @@
       <c r="E34" s="5"/>
       <c r="F34" s="5"/>
       <c r="G34" s="5"/>
-      <c r="H34" s="21" t="s">
+      <c r="H34" s="15" t="s">
         <v>10</v>
       </c>
       <c r="I34" s="5"/>
@@ -1534,10 +1687,10 @@
       <c r="L34" s="5"/>
       <c r="M34" s="5"/>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A35" s="18"/>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A35" s="19"/>
       <c r="B35" s="13" t="s">
-        <v>43</v>
+        <v>74</v>
       </c>
       <c r="C35" s="13" t="s">
         <v>13</v>
@@ -1545,22 +1698,22 @@
       <c r="D35" s="5"/>
       <c r="E35" s="5"/>
       <c r="F35" s="5"/>
-      <c r="G35" s="21" t="s">
+      <c r="G35" s="15" t="s">
         <v>10</v>
       </c>
       <c r="H35" s="5"/>
       <c r="I35" s="5"/>
-      <c r="J35" s="21" t="s">
+      <c r="J35" s="15" t="s">
         <v>10</v>
       </c>
       <c r="K35" s="5"/>
       <c r="L35" s="5"/>
       <c r="M35" s="5"/>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A36" s="18"/>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A36" s="19"/>
       <c r="B36" s="13" t="s">
-        <v>44</v>
+        <v>75</v>
       </c>
       <c r="C36" s="13" t="s">
         <v>13</v>
@@ -1568,7 +1721,7 @@
       <c r="D36" s="5"/>
       <c r="E36" s="5"/>
       <c r="F36" s="5"/>
-      <c r="G36" s="21" t="s">
+      <c r="G36" s="15" t="s">
         <v>10</v>
       </c>
       <c r="H36" s="5"/>
@@ -1578,10 +1731,10 @@
       <c r="L36" s="5"/>
       <c r="M36" s="5"/>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A37" s="18"/>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A37" s="19"/>
       <c r="B37" s="13" t="s">
-        <v>45</v>
+        <v>76</v>
       </c>
       <c r="C37" s="13" t="s">
         <v>13</v>
@@ -1592,22 +1745,22 @@
       <c r="G37" s="5"/>
       <c r="H37" s="5"/>
       <c r="I37" s="5"/>
-      <c r="J37" s="21" t="s">
+      <c r="J37" s="15" t="s">
         <v>10</v>
       </c>
       <c r="K37" s="5"/>
       <c r="L37" s="5"/>
       <c r="M37" s="5"/>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A38" s="18"/>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A38" s="19"/>
       <c r="B38" s="13" t="s">
-        <v>46</v>
+        <v>77</v>
       </c>
       <c r="C38" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="D38" s="21" t="s">
+      <c r="D38" s="15" t="s">
         <v>10</v>
       </c>
       <c r="E38" s="5"/>
@@ -1620,10 +1773,10 @@
       <c r="L38" s="5"/>
       <c r="M38" s="5"/>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A39" s="18"/>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A39" s="19"/>
       <c r="B39" s="14" t="s">
-        <v>47</v>
+        <v>78</v>
       </c>
       <c r="C39" s="14" t="s">
         <v>13</v>
@@ -1645,10 +1798,10 @@
       <c r="L39" s="5"/>
       <c r="M39" s="5"/>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A40" s="18"/>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A40" s="19"/>
       <c r="B40" s="14" t="s">
-        <v>48</v>
+        <v>79</v>
       </c>
       <c r="C40" s="14" t="s">
         <v>13</v>
@@ -1668,10 +1821,10 @@
       <c r="L40" s="5"/>
       <c r="M40" s="5"/>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A41" s="18"/>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A41" s="19"/>
       <c r="B41" s="14" t="s">
-        <v>49</v>
+        <v>80</v>
       </c>
       <c r="C41" s="14" t="s">
         <v>13</v>
@@ -1689,10 +1842,10 @@
       <c r="L41" s="5"/>
       <c r="M41" s="5"/>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A42" s="18"/>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A42" s="19"/>
       <c r="B42" s="14" t="s">
-        <v>50</v>
+        <v>81</v>
       </c>
       <c r="C42" s="14" t="s">
         <v>13</v>
@@ -1712,17 +1865,23 @@
       <c r="L42" s="5"/>
       <c r="M42" s="5"/>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A43" s="18"/>
-      <c r="B43" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C43" s="1" t="s">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A43" s="19"/>
+      <c r="B43" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="C43" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="D43" s="5"/>
-      <c r="E43" s="5"/>
-      <c r="F43" s="5"/>
+      <c r="D43" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="E43" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="F43" s="28" t="s">
+        <v>10</v>
+      </c>
       <c r="G43" s="5"/>
       <c r="H43" s="5"/>
       <c r="I43" s="5"/>
@@ -1731,16 +1890,18 @@
       <c r="L43" s="5"/>
       <c r="M43" s="5"/>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A44" s="18"/>
-      <c r="B44" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C44" s="1" t="s">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A44" s="19"/>
+      <c r="B44" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="C44" s="21" t="s">
         <v>14</v>
       </c>
       <c r="D44" s="5"/>
-      <c r="E44" s="5"/>
+      <c r="E44" s="28" t="s">
+        <v>10</v>
+      </c>
       <c r="F44" s="5"/>
       <c r="G44" s="5"/>
       <c r="H44" s="5"/>
@@ -1750,17 +1911,19 @@
       <c r="L44" s="5"/>
       <c r="M44" s="5"/>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A45" s="18"/>
-      <c r="B45" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>15</v>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A45" s="19"/>
+      <c r="B45" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="C45" s="21" t="s">
+        <v>14</v>
       </c>
       <c r="D45" s="5"/>
       <c r="E45" s="5"/>
-      <c r="F45" s="5"/>
+      <c r="F45" s="28" t="s">
+        <v>10</v>
+      </c>
       <c r="G45" s="5"/>
       <c r="H45" s="5"/>
       <c r="I45" s="5"/>
@@ -1769,17 +1932,23 @@
       <c r="L45" s="5"/>
       <c r="M45" s="5"/>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A46" s="19"/>
-      <c r="B46" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C46" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D46" s="5"/>
-      <c r="E46" s="5"/>
-      <c r="F46" s="5"/>
+      <c r="B46" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="C46" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="D46" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="E46" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="F46" s="28" t="s">
+        <v>10</v>
+      </c>
       <c r="G46" s="5"/>
       <c r="H46" s="5"/>
       <c r="I46" s="5"/>
@@ -1788,14 +1957,563 @@
       <c r="L46" s="5"/>
       <c r="M46" s="5"/>
     </row>
-    <row r="51" spans="7:7" x14ac:dyDescent="0.3">
-      <c r="G51" s="4"/>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A47" s="19"/>
+      <c r="B47" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="C47" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="D47" s="5"/>
+      <c r="E47" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="F47" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="G47" s="5"/>
+      <c r="H47" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="I47" s="5"/>
+      <c r="J47" s="5"/>
+      <c r="K47" s="5"/>
+      <c r="L47" s="5"/>
+      <c r="M47" s="5"/>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A48" s="19"/>
+      <c r="B48" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="C48" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="D48" s="5"/>
+      <c r="E48" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="F48" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="G48" s="5"/>
+      <c r="H48" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="I48" s="5"/>
+      <c r="J48" s="5"/>
+      <c r="K48" s="5"/>
+      <c r="L48" s="5"/>
+      <c r="M48" s="5"/>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A49" s="19"/>
+      <c r="B49" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="C49" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="D49" s="5"/>
+      <c r="E49" s="5"/>
+      <c r="F49" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="G49" s="5"/>
+      <c r="H49" s="5"/>
+      <c r="I49" s="5"/>
+      <c r="J49" s="5"/>
+      <c r="K49" s="5"/>
+      <c r="L49" s="5"/>
+      <c r="M49" s="5"/>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A50" s="19"/>
+      <c r="B50" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="C50" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="D50" s="5"/>
+      <c r="E50" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="F50" s="5"/>
+      <c r="G50" s="5"/>
+      <c r="H50" s="5"/>
+      <c r="I50" s="5"/>
+      <c r="J50" s="5"/>
+      <c r="K50" s="5"/>
+      <c r="L50" s="5"/>
+      <c r="M50" s="5"/>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A51" s="19"/>
+      <c r="B51" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="C51" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="D51" s="5"/>
+      <c r="E51" s="5"/>
+      <c r="F51" s="5"/>
+      <c r="G51" s="5"/>
+      <c r="H51" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="I51" s="5"/>
+      <c r="J51" s="5"/>
+      <c r="K51" s="5"/>
+      <c r="L51" s="5"/>
+      <c r="M51" s="5"/>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A52" s="19"/>
+      <c r="B52" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="C52" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="D52" s="5"/>
+      <c r="E52" s="5"/>
+      <c r="F52" s="5"/>
+      <c r="G52" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="H52" s="5"/>
+      <c r="I52" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="J52" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="K52" s="5"/>
+      <c r="L52" s="5"/>
+      <c r="M52" s="5"/>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A53" s="19"/>
+      <c r="B53" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="C53" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="D53" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="E53" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="F53" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="G53" s="5"/>
+      <c r="H53" s="5"/>
+      <c r="I53" s="5"/>
+      <c r="J53" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="K53" s="5"/>
+      <c r="L53" s="5"/>
+      <c r="M53" s="5"/>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A54" s="19"/>
+      <c r="B54" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="C54" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="D54" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="E54" s="5"/>
+      <c r="F54" s="5"/>
+      <c r="G54" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="H54" s="5"/>
+      <c r="I54" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="J54" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="K54" s="5"/>
+      <c r="L54" s="5"/>
+      <c r="M54" s="5"/>
+    </row>
+    <row r="55" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A55" s="19"/>
+      <c r="B55" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D55" s="5"/>
+      <c r="E55" s="5"/>
+      <c r="F55" s="5"/>
+      <c r="G55" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="H55" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="I55" s="5"/>
+      <c r="J55" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="K55" s="5"/>
+      <c r="L55" s="5"/>
+      <c r="M55" s="5"/>
+    </row>
+    <row r="56" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A56" s="19"/>
+      <c r="B56" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D56" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="E56" s="5"/>
+      <c r="F56" s="5"/>
+      <c r="G56" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="H56" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="I56" s="5"/>
+      <c r="J56" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="K56" s="5"/>
+      <c r="L56" s="5"/>
+      <c r="M56" s="5"/>
+    </row>
+    <row r="57" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A57" s="19"/>
+      <c r="B57" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D57" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="E57" s="5"/>
+      <c r="F57" s="5"/>
+      <c r="G57" s="5"/>
+      <c r="H57" s="5"/>
+      <c r="I57" s="5"/>
+      <c r="J57" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="K57" s="5"/>
+      <c r="L57" s="5"/>
+      <c r="M57" s="5"/>
+    </row>
+    <row r="58" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A58" s="19"/>
+      <c r="B58" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D58" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="E58" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="F58" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="G58" s="5"/>
+      <c r="H58" s="5"/>
+      <c r="I58" s="5"/>
+      <c r="J58" s="5"/>
+      <c r="K58" s="5"/>
+      <c r="L58" s="5"/>
+      <c r="M58" s="5"/>
+    </row>
+    <row r="59" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A59" s="19"/>
+      <c r="B59" s="23" t="s">
+        <v>41</v>
+      </c>
+      <c r="C59" s="23" t="s">
+        <v>92</v>
+      </c>
+      <c r="D59" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E59" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F59" s="5"/>
+      <c r="G59" s="5"/>
+      <c r="H59" s="5"/>
+      <c r="I59" s="5"/>
+      <c r="J59" s="5"/>
+      <c r="K59" s="5"/>
+      <c r="L59" s="5"/>
+      <c r="M59" s="5"/>
+    </row>
+    <row r="60" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A60" s="19"/>
+      <c r="B60" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="C60" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="D60" s="5"/>
+      <c r="E60" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F60" s="5"/>
+      <c r="G60" s="5"/>
+      <c r="H60" s="5"/>
+      <c r="I60" s="5"/>
+      <c r="J60" s="5"/>
+      <c r="K60" s="5"/>
+      <c r="L60" s="5"/>
+      <c r="M60" s="5"/>
+    </row>
+    <row r="61" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A61" s="19"/>
+      <c r="B61" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="C61" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="D61" s="5"/>
+      <c r="E61" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F61" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G61" s="5"/>
+      <c r="H61" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="I61" s="5"/>
+      <c r="J61" s="5"/>
+      <c r="K61" s="5"/>
+      <c r="L61" s="5"/>
+      <c r="M61" s="5"/>
+    </row>
+    <row r="62" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A62" s="19"/>
+      <c r="B62" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="C62" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="D62" s="5"/>
+      <c r="E62" s="5"/>
+      <c r="F62" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G62" s="5"/>
+      <c r="H62" s="5"/>
+      <c r="I62" s="5"/>
+      <c r="J62" s="5"/>
+      <c r="K62" s="5"/>
+      <c r="L62" s="5"/>
+      <c r="M62" s="5"/>
+    </row>
+    <row r="63" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A63" s="19"/>
+      <c r="B63" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="C63" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="D63" s="5"/>
+      <c r="E63" s="5"/>
+      <c r="F63" s="5"/>
+      <c r="G63" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H63" s="5"/>
+      <c r="I63" s="5"/>
+      <c r="J63" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="K63" s="5"/>
+      <c r="L63" s="5"/>
+      <c r="M63" s="5"/>
+    </row>
+    <row r="64" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A64" s="19"/>
+      <c r="B64" s="24" t="s">
+        <v>86</v>
+      </c>
+      <c r="C64" s="24" t="s">
+        <v>92</v>
+      </c>
+      <c r="D64" s="5"/>
+      <c r="E64" s="5"/>
+      <c r="F64" s="5"/>
+      <c r="G64" s="5"/>
+      <c r="H64" s="5"/>
+      <c r="I64" s="5"/>
+      <c r="J64" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="K64" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="L64" s="5"/>
+      <c r="M64" s="5"/>
+    </row>
+    <row r="65" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A65" s="19"/>
+      <c r="B65" s="24" t="s">
+        <v>87</v>
+      </c>
+      <c r="C65" s="24" t="s">
+        <v>92</v>
+      </c>
+      <c r="D65" s="5"/>
+      <c r="E65" s="5"/>
+      <c r="F65" s="5"/>
+      <c r="G65" s="5"/>
+      <c r="H65" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="I65" s="5"/>
+      <c r="J65" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="K65" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="L65" s="5"/>
+      <c r="M65" s="5"/>
+    </row>
+    <row r="66" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A66" s="19"/>
+      <c r="B66" s="24" t="s">
+        <v>88</v>
+      </c>
+      <c r="C66" s="24" t="s">
+        <v>92</v>
+      </c>
+      <c r="D66" s="5"/>
+      <c r="E66" s="5"/>
+      <c r="F66" s="5"/>
+      <c r="G66" s="5"/>
+      <c r="H66" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="I66" s="5"/>
+      <c r="J66" s="5"/>
+      <c r="K66" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="L66" s="5"/>
+      <c r="M66" s="5"/>
+    </row>
+    <row r="67" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A67" s="19"/>
+      <c r="B67" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="C67" s="25" t="s">
+        <v>92</v>
+      </c>
+      <c r="D67" s="5"/>
+      <c r="E67" s="5"/>
+      <c r="F67" s="5"/>
+      <c r="G67" s="5"/>
+      <c r="H67" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="I67" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="J67" s="5"/>
+      <c r="K67" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="L67" s="5"/>
+      <c r="M67" s="5"/>
+    </row>
+    <row r="68" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A68" s="19"/>
+      <c r="B68" s="26" t="s">
+        <v>90</v>
+      </c>
+      <c r="C68" s="26" t="s">
+        <v>92</v>
+      </c>
+      <c r="D68" s="5"/>
+      <c r="E68" s="5"/>
+      <c r="F68" s="5"/>
+      <c r="G68" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H68" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="I68" s="5"/>
+      <c r="J68" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="K68" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="L68" s="5"/>
+      <c r="M68" s="5"/>
+    </row>
+    <row r="69" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A69" s="19"/>
+      <c r="B69" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="C69" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="D69" s="5"/>
+      <c r="E69" s="5"/>
+      <c r="F69" s="5"/>
+      <c r="G69" s="5"/>
+      <c r="H69" s="5"/>
+      <c r="I69" s="5"/>
+      <c r="J69" s="5"/>
+      <c r="K69" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="L69" s="5"/>
+      <c r="M69" s="5"/>
+    </row>
+    <row r="74" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="G74" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="D1:M1"/>
-    <mergeCell ref="A3:A46"/>
+    <mergeCell ref="A3:A69"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="B1:B2"/>
   </mergeCells>

</xml_diff>